<commit_message>
Proyecto final terminado version 1
</commit_message>
<xml_diff>
--- a/assets/excel/Nuevo_Hoja_de_calculo_de_Microsoft_Excel.xlsx
+++ b/assets/excel/Nuevo_Hoja_de_calculo_de_Microsoft_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j-mar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyectico_v2\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D717429-CDC4-485E-8C4E-B85115B19FBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5A80C2-AA38-40E8-8E7F-BC7AE3891CCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,78 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Vargaz</t>
   </si>
   <si>
-    <t>xde</t>
-  </si>
-  <si>
-    <t>dede</t>
-  </si>
-  <si>
-    <t>iaka</t>
-  </si>
-  <si>
-    <t>penagos</t>
-  </si>
-  <si>
-    <t>mario</t>
-  </si>
-  <si>
-    <t>arteria</t>
-  </si>
-  <si>
-    <t>sebas</t>
-  </si>
-  <si>
-    <t>stewen</t>
-  </si>
-  <si>
-    <t>erik</t>
-  </si>
-  <si>
-    <t>nigg</t>
-  </si>
-  <si>
-    <t>blank</t>
-  </si>
-  <si>
-    <t>mario@hotmail.com</t>
-  </si>
-  <si>
-    <t>arteria@hotmail.com</t>
-  </si>
-  <si>
-    <t>sebas@hotmail.com</t>
-  </si>
-  <si>
-    <t>iaka@gmail.com</t>
-  </si>
-  <si>
-    <t>stewen@gmail.com</t>
-  </si>
-  <si>
-    <t>erik@gmail.com</t>
-  </si>
-  <si>
-    <t>alegria</t>
-  </si>
-  <si>
-    <t>vladimir</t>
-  </si>
-  <si>
-    <t>ssassa</t>
-  </si>
-  <si>
-    <t>dd3wdd</t>
-  </si>
-  <si>
-    <t>alergico@hotmail.com</t>
-  </si>
-  <si>
-    <t>vlacho@hotmail.com</t>
+    <t xml:space="preserve">Jorge Mario </t>
+  </si>
+  <si>
+    <t>Sebastian Morales</t>
+  </si>
+  <si>
+    <t>Barrientos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erik Stiven </t>
+  </si>
+  <si>
+    <t>Alegria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eduard </t>
+  </si>
+  <si>
+    <t>Gil Lozada</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Rodrigues</t>
+  </si>
+  <si>
+    <t>Isabela</t>
+  </si>
+  <si>
+    <t>Landazuri</t>
+  </si>
+  <si>
+    <t>Landazuri@gmail.com</t>
+  </si>
+  <si>
+    <t>Rodrigues@gmail.com</t>
+  </si>
+  <si>
+    <t>Lozada@gmail.com</t>
+  </si>
+  <si>
+    <t>Alegria@hotmail.com</t>
+  </si>
+  <si>
+    <t>Barrientos@hotmail.com</t>
+  </si>
+  <si>
+    <t>Vargaz@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -149,11 +131,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -435,140 +416,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>6845123</v>
+        <v>123451</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>4564512</v>
+        <v>123452</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>6489122</v>
+        <v>123453</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>21651233</v>
+        <v>123454</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>215465</v>
+        <v>123455</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>9513006</v>
+        <v>123456</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>5642135</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>9851231</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -578,10 +531,8 @@
     <hyperlink ref="D3" r:id="rId4" xr:uid="{FB2A8DAA-5640-4200-9822-9E65BA21BBC1}"/>
     <hyperlink ref="D2" r:id="rId5" xr:uid="{C9ED5669-F295-402C-B7E0-E75F8969A1B6}"/>
     <hyperlink ref="D4" r:id="rId6" xr:uid="{F57992C3-4482-4F72-8079-28A79D29F3B9}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{3B0A869E-B991-4E70-84B8-032D7CE012BF}"/>
-    <hyperlink ref="D8" r:id="rId8" xr:uid="{FFFD6F44-DBF3-414A-ABC9-755F3636F951}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>